<commit_message>
commit before updating my data file
</commit_message>
<xml_diff>
--- a/time spacing/words_V1.0.0.xlsx
+++ b/time spacing/words_V1.0.0.xlsx
@@ -440,7 +440,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="2">
@@ -455,10 +455,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45330</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="3">
@@ -473,10 +473,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>45325</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="4">
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>45320</v>
+        <v>45356</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +512,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="6">
@@ -530,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="7">
@@ -548,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="8">
@@ -566,7 +566,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>45334</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="9">
@@ -602,7 +602,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="11">
@@ -620,7 +620,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="12">
@@ -638,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="13">
@@ -653,10 +653,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>45320</v>
+        <v>45353</v>
       </c>
     </row>
     <row r="14">
@@ -674,7 +674,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>45324</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="15">
@@ -689,10 +689,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>45321</v>
+        <v>45368</v>
       </c>
     </row>
     <row r="16">
@@ -707,10 +707,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>45320</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="17">
@@ -725,10 +725,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>45320</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="18">
@@ -761,10 +761,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="20">
@@ -782,7 +782,7 @@
         <v>8</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="21">
@@ -815,10 +815,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="23">
@@ -836,7 +836,7 @@
         <v>16</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="24">
@@ -851,10 +851,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>45324</v>
+        <v>45367</v>
       </c>
     </row>
     <row r="25">
@@ -869,10 +869,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>45321</v>
+        <v>45366</v>
       </c>
     </row>
     <row r="26">
@@ -905,10 +905,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>45320</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="28">
@@ -923,10 +923,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>45337</v>
+        <v>45401</v>
       </c>
     </row>
     <row r="29">
@@ -941,10 +941,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>45330</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="30">
@@ -962,7 +962,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="31">
@@ -980,7 +980,7 @@
         <v>16</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="32">
@@ -1013,10 +1013,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="34">
@@ -1031,10 +1031,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>45320</v>
+        <v>45342</v>
       </c>
     </row>
     <row r="35">
@@ -1049,10 +1049,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>45320</v>
+        <v>45349</v>
       </c>
     </row>
     <row r="36">
@@ -1067,10 +1067,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="37">
@@ -1085,10 +1085,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>45321</v>
+        <v>45353</v>
       </c>
     </row>
     <row r="38">
@@ -1103,10 +1103,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>45330</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="39">
@@ -1124,7 +1124,7 @@
         <v>4</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="40">
@@ -1142,7 +1142,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="41">
@@ -1157,10 +1157,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>45320</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="42">
@@ -1178,7 +1178,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="43">
@@ -1196,7 +1196,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="44">
@@ -1229,10 +1229,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>45322</v>
+        <v>45368</v>
       </c>
     </row>
     <row r="46">
@@ -1250,7 +1250,7 @@
         <v>16</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="47">
@@ -1268,7 +1268,7 @@
         <v>8</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="48">
@@ -1283,10 +1283,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>45326</v>
+        <v>45346</v>
       </c>
     </row>
     <row r="49">
@@ -1301,10 +1301,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>45320</v>
+        <v>45353</v>
       </c>
     </row>
     <row r="50">
@@ -1319,10 +1319,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="51">
@@ -1340,7 +1340,7 @@
         <v>4</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="52">
@@ -1358,7 +1358,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="53">
@@ -1376,7 +1376,7 @@
         <v>16</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="54">
@@ -1391,10 +1391,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>45321</v>
+        <v>45354</v>
       </c>
     </row>
     <row r="55">
@@ -1409,10 +1409,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>45320</v>
+        <v>45345</v>
       </c>
     </row>
     <row r="56">
@@ -1427,10 +1427,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>45325</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="57">
@@ -1445,10 +1445,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>45330</v>
+        <v>45395</v>
       </c>
     </row>
     <row r="58">
@@ -1481,10 +1481,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>45323</v>
+        <v>45345</v>
       </c>
     </row>
     <row r="60">
@@ -1499,10 +1499,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>45334</v>
+        <v>45366</v>
       </c>
     </row>
     <row r="61">
@@ -1520,7 +1520,7 @@
         <v>8</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="62">
@@ -1535,10 +1535,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>45332</v>
+        <v>45398</v>
       </c>
     </row>
     <row r="63">
@@ -1553,10 +1553,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>45320</v>
+        <v>45340</v>
       </c>
     </row>
     <row r="64">
@@ -1571,10 +1571,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>45325</v>
+        <v>45357</v>
       </c>
     </row>
     <row r="65">
@@ -1589,10 +1589,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>45320</v>
+        <v>45352</v>
       </c>
     </row>
     <row r="66">
@@ -1607,10 +1607,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>45326</v>
+        <v>45350</v>
       </c>
     </row>
     <row r="67">
@@ -1625,10 +1625,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>45320</v>
+        <v>45349</v>
       </c>
     </row>
     <row r="68">
@@ -1643,10 +1643,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>45320</v>
+        <v>45352</v>
       </c>
     </row>
     <row r="69">
@@ -1661,10 +1661,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>45330</v>
+        <v>45366</v>
       </c>
     </row>
     <row r="70">
@@ -1682,7 +1682,7 @@
         <v>2</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="71">
@@ -1697,10 +1697,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>45320</v>
+        <v>45350</v>
       </c>
     </row>
     <row r="72">
@@ -1718,7 +1718,7 @@
         <v>32</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>45335</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="73">
@@ -1736,7 +1736,7 @@
         <v>8</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="74">
@@ -1754,7 +1754,7 @@
         <v>2</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="75">
@@ -1772,7 +1772,7 @@
         <v>2</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="76">
@@ -1787,10 +1787,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="77">
@@ -1805,10 +1805,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>45322</v>
+        <v>45362</v>
       </c>
     </row>
     <row r="78">
@@ -1826,7 +1826,7 @@
         <v>16</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>45335</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="79">
@@ -1841,10 +1841,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>45320</v>
+        <v>45354</v>
       </c>
     </row>
     <row r="80">
@@ -1877,10 +1877,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>45323</v>
+        <v>45358</v>
       </c>
     </row>
     <row r="82">
@@ -1898,7 +1898,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="83">
@@ -1913,10 +1913,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>45320</v>
+        <v>45353</v>
       </c>
     </row>
     <row r="84">
@@ -1934,7 +1934,7 @@
         <v>4</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="85">
@@ -1949,10 +1949,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="86">
@@ -1970,7 +1970,7 @@
         <v>2</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="87">
@@ -1985,10 +1985,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>45321</v>
+        <v>45362</v>
       </c>
     </row>
     <row r="88">
@@ -2006,7 +2006,7 @@
         <v>16</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="89">
@@ -2024,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="90">
@@ -2039,10 +2039,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>45320</v>
+        <v>45342</v>
       </c>
     </row>
     <row r="91">
@@ -2057,10 +2057,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D91" s="1" t="n">
-        <v>45324</v>
+        <v>45365</v>
       </c>
     </row>
     <row r="92">
@@ -2075,10 +2075,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D92" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="93">
@@ -2096,7 +2096,7 @@
         <v>8</v>
       </c>
       <c r="D93" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="94">
@@ -2114,7 +2114,7 @@
         <v>8</v>
       </c>
       <c r="D94" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="95">
@@ -2129,10 +2129,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D95" s="1" t="n">
-        <v>45321</v>
+        <v>45345</v>
       </c>
     </row>
     <row r="96">
@@ -2150,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="97">
@@ -2168,7 +2168,7 @@
         <v>4</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="98">
@@ -2183,10 +2183,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>45320</v>
+        <v>45349</v>
       </c>
     </row>
     <row r="99">
@@ -2204,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="100">
@@ -2222,7 +2222,7 @@
         <v>16</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>45336</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="101">
@@ -2240,7 +2240,7 @@
         <v>2</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="102">
@@ -2258,7 +2258,7 @@
         <v>4</v>
       </c>
       <c r="D102" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="103">
@@ -2273,10 +2273,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D103" s="1" t="n">
-        <v>45320</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="104">
@@ -2294,7 +2294,7 @@
         <v>8</v>
       </c>
       <c r="D104" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="105">
@@ -2312,7 +2312,7 @@
         <v>2</v>
       </c>
       <c r="D105" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="106">
@@ -2327,10 +2327,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D106" s="1" t="n">
-        <v>45320</v>
+        <v>45349</v>
       </c>
     </row>
     <row r="107">
@@ -2363,10 +2363,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>45320</v>
+        <v>45342</v>
       </c>
     </row>
     <row r="109">
@@ -2381,10 +2381,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>45320</v>
+        <v>45339</v>
       </c>
     </row>
     <row r="110">
@@ -2402,7 +2402,7 @@
         <v>2</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="111">
@@ -2420,7 +2420,7 @@
         <v>4</v>
       </c>
       <c r="D111" s="1" t="n">
-        <v>45324</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="112">
@@ -2435,10 +2435,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>45320</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="113">
@@ -2453,10 +2453,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>45320</v>
+        <v>45345</v>
       </c>
     </row>
     <row r="114">
@@ -2474,7 +2474,7 @@
         <v>16</v>
       </c>
       <c r="D114" s="1" t="n">
-        <v>45324</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="115">
@@ -2492,7 +2492,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="116">
@@ -2510,7 +2510,7 @@
         <v>8</v>
       </c>
       <c r="D116" s="1" t="n">
-        <v>45327</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="117">
@@ -2528,7 +2528,7 @@
         <v>4</v>
       </c>
       <c r="D117" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="118">
@@ -2543,10 +2543,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D118" s="1" t="n">
-        <v>45320</v>
+        <v>45347</v>
       </c>
     </row>
     <row r="119">
@@ -2561,10 +2561,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D119" s="1" t="n">
-        <v>45328</v>
+        <v>45366</v>
       </c>
     </row>
     <row r="120">
@@ -2582,7 +2582,7 @@
         <v>16</v>
       </c>
       <c r="D120" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="121">
@@ -2597,10 +2597,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D121" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="122">
@@ -2618,7 +2618,7 @@
         <v>16</v>
       </c>
       <c r="D122" s="1" t="n">
-        <v>45325</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="123">
@@ -2633,10 +2633,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D123" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="124">
@@ -2654,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="D124" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="125">
@@ -2669,10 +2669,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D125" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="126">
@@ -2687,10 +2687,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D126" s="1" t="n">
-        <v>45334</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="127">
@@ -2705,10 +2705,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D127" s="1" t="n">
-        <v>45320</v>
+        <v>45354</v>
       </c>
     </row>
     <row r="128">
@@ -2723,10 +2723,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D128" s="1" t="n">
-        <v>45320</v>
+        <v>45352</v>
       </c>
     </row>
     <row r="129">
@@ -2744,7 +2744,7 @@
         <v>8</v>
       </c>
       <c r="D129" s="1" t="n">
-        <v>45327</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="130">
@@ -2759,10 +2759,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D130" s="1" t="n">
-        <v>45321</v>
+        <v>45356</v>
       </c>
     </row>
     <row r="131">
@@ -2777,10 +2777,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D131" s="1" t="n">
-        <v>45320</v>
+        <v>45345</v>
       </c>
     </row>
     <row r="132">
@@ -2795,10 +2795,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D132" s="1" t="n">
-        <v>45320</v>
+        <v>45352</v>
       </c>
     </row>
     <row r="133">
@@ -2813,10 +2813,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D133" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="134">
@@ -2834,7 +2834,7 @@
         <v>4</v>
       </c>
       <c r="D134" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="135">
@@ -2849,10 +2849,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D135" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="136">
@@ -2873,7 +2873,7 @@
         <v>1</v>
       </c>
       <c r="D136" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="137">
@@ -2888,10 +2888,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D137" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="138">
@@ -2906,10 +2906,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D138" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="139">
@@ -2927,7 +2927,7 @@
         <v>1</v>
       </c>
       <c r="D139" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="140">
@@ -2943,10 +2943,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D140" s="1" t="n">
-        <v>45320</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="141">
@@ -2966,7 +2966,7 @@
         <v>4</v>
       </c>
       <c r="D141" s="1" t="n">
-        <v>45324</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="142">
@@ -2983,10 +2983,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D142" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="143">
@@ -3006,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="D143" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="144">
@@ -3024,7 +3024,7 @@
         <v>2</v>
       </c>
       <c r="D144" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="145">
@@ -3039,10 +3039,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D145" s="1" t="n">
-        <v>45328</v>
+        <v>45350</v>
       </c>
     </row>
     <row r="146">
@@ -3061,7 +3061,7 @@
         <v>1</v>
       </c>
       <c r="D146" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="147">
@@ -3078,10 +3078,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D147" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="148">
@@ -3096,10 +3096,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D148" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="149">
@@ -3114,10 +3114,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D149" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="150">
@@ -3132,10 +3132,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D150" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="151">
@@ -3154,7 +3154,7 @@
         <v>8</v>
       </c>
       <c r="D151" s="1" t="n">
-        <v>45328</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="152">
@@ -3173,7 +3173,7 @@
         <v>2</v>
       </c>
       <c r="D152" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="153">
@@ -3192,7 +3192,7 @@
         <v>1</v>
       </c>
       <c r="D153" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="154">
@@ -3207,10 +3207,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D154" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="155">
@@ -3228,7 +3228,7 @@
         <v>1</v>
       </c>
       <c r="D155" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="156">
@@ -3247,7 +3247,7 @@
         <v>2</v>
       </c>
       <c r="D156" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="157">
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D157" s="1" t="n">
-        <v>45320</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="158">
@@ -3284,7 +3284,7 @@
         <v>1</v>
       </c>
       <c r="D158" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="159">
@@ -3301,10 +3301,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D159" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="160">
@@ -3323,7 +3323,7 @@
         <v>1</v>
       </c>
       <c r="D160" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="161">
@@ -3342,7 +3342,7 @@
         <v>2</v>
       </c>
       <c r="D161" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="162">
@@ -3360,7 +3360,7 @@
         <v>1</v>
       </c>
       <c r="D162" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="163">
@@ -3375,10 +3375,10 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D163" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="164">
@@ -3396,7 +3396,7 @@
         <v>2</v>
       </c>
       <c r="D164" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="165">
@@ -3414,7 +3414,7 @@
         <v>1</v>
       </c>
       <c r="D165" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="166">
@@ -3432,7 +3432,7 @@
         <v>2</v>
       </c>
       <c r="D166" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="167">
@@ -3451,7 +3451,7 @@
         <v>1</v>
       </c>
       <c r="D167" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="168">
@@ -3466,10 +3466,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D168" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="169">
@@ -3484,10 +3484,10 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D169" s="1" t="n">
-        <v>45324</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="170">
@@ -3506,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="D170" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="171">
@@ -3524,7 +3524,7 @@
         <v>1</v>
       </c>
       <c r="D171" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="172">
@@ -3542,7 +3542,7 @@
         <v>1</v>
       </c>
       <c r="D172" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="173">
@@ -3560,7 +3560,7 @@
         <v>4</v>
       </c>
       <c r="D173" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="174">
@@ -3575,10 +3575,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D174" s="1" t="n">
-        <v>45328</v>
+        <v>45352</v>
       </c>
     </row>
     <row r="175">
@@ -3596,7 +3596,7 @@
         <v>4</v>
       </c>
       <c r="D175" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="176">
@@ -3614,7 +3614,7 @@
         <v>4</v>
       </c>
       <c r="D176" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="177">
@@ -3629,10 +3629,10 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D177" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="178">
@@ -3650,7 +3650,7 @@
         <v>2</v>
       </c>
       <c r="D178" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="179">
@@ -3665,10 +3665,10 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D179" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="180">
@@ -3686,7 +3686,7 @@
         <v>4</v>
       </c>
       <c r="D180" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="181">
@@ -3701,10 +3701,10 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D181" s="1" t="n">
-        <v>45320</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="182">
@@ -3722,7 +3722,7 @@
         <v>2</v>
       </c>
       <c r="D182" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="183">
@@ -3740,7 +3740,7 @@
         <v>1</v>
       </c>
       <c r="D183" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="184">
@@ -3759,7 +3759,7 @@
         <v>2</v>
       </c>
       <c r="D184" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="185">
@@ -3777,7 +3777,7 @@
         <v>4</v>
       </c>
       <c r="D185" s="1" t="n">
-        <v>45323</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="186">
@@ -3792,10 +3792,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D186" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="187">
@@ -3810,10 +3810,10 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D187" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="188">
@@ -3828,10 +3828,10 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D188" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="189">
@@ -3849,7 +3849,7 @@
         <v>2</v>
       </c>
       <c r="D189" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="190">
@@ -3864,10 +3864,10 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D190" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="191">
@@ -3882,10 +3882,10 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D191" s="1" t="n">
-        <v>45320</v>
+        <v>45339</v>
       </c>
     </row>
     <row r="192">
@@ -3900,10 +3900,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D192" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="193">
@@ -3918,10 +3918,10 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D193" s="1" t="n">
-        <v>45320</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="194">
@@ -3937,10 +3937,10 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D194" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="195">
@@ -3955,10 +3955,10 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D195" s="1" t="n">
-        <v>45320</v>
+        <v>45340</v>
       </c>
     </row>
     <row r="196">
@@ -3973,10 +3973,10 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D196" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="197">
@@ -3991,10 +3991,10 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D197" s="1" t="n">
-        <v>45320</v>
+        <v>45352</v>
       </c>
     </row>
     <row r="198">
@@ -4009,10 +4009,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D198" s="1" t="n">
-        <v>45320</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="199">
@@ -4027,10 +4027,10 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D199" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="200">
@@ -4048,7 +4048,7 @@
         <v>1</v>
       </c>
       <c r="D200" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="201">
@@ -4063,10 +4063,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D201" s="1" t="n">
-        <v>45320</v>
+        <v>45340</v>
       </c>
     </row>
     <row r="202">
@@ -4084,7 +4084,7 @@
         <v>1</v>
       </c>
       <c r="D202" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="203">
@@ -4102,7 +4102,7 @@
         <v>1</v>
       </c>
       <c r="D203" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="204">
@@ -4120,7 +4120,7 @@
         <v>1</v>
       </c>
       <c r="D204" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="205">
@@ -4138,7 +4138,7 @@
         <v>1</v>
       </c>
       <c r="D205" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="206">
@@ -4156,7 +4156,7 @@
         <v>1</v>
       </c>
       <c r="D206" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="207">
@@ -4174,7 +4174,7 @@
         <v>1</v>
       </c>
       <c r="D207" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="208">
@@ -4192,7 +4192,7 @@
         <v>1</v>
       </c>
       <c r="D208" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="209">
@@ -4207,10 +4207,10 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D209" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="210">
@@ -4225,10 +4225,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D210" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="211">
@@ -4243,10 +4243,10 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D211" s="1" t="n">
-        <v>45324</v>
+        <v>45339</v>
       </c>
     </row>
     <row r="212">
@@ -4261,10 +4261,10 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D212" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="213">
@@ -4279,10 +4279,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D213" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="214">
@@ -4297,10 +4297,10 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D214" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="215">
@@ -4318,7 +4318,7 @@
         <v>1</v>
       </c>
       <c r="D215" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="216">
@@ -4336,7 +4336,7 @@
         <v>1</v>
       </c>
       <c r="D216" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="217">
@@ -4356,7 +4356,7 @@
         <v>1</v>
       </c>
       <c r="D217" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="218">
@@ -4371,10 +4371,10 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D218" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="219">
@@ -4389,10 +4389,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D219" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="220">
@@ -4410,7 +4410,7 @@
         <v>1</v>
       </c>
       <c r="D220" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="221">
@@ -4425,10 +4425,10 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D221" s="1" t="n">
-        <v>45320</v>
+        <v>45345</v>
       </c>
     </row>
     <row r="222">
@@ -4447,7 +4447,7 @@
         <v>1</v>
       </c>
       <c r="D222" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="223">
@@ -4465,7 +4465,7 @@
         <v>1</v>
       </c>
       <c r="D223" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="224">
@@ -4483,7 +4483,7 @@
         <v>1</v>
       </c>
       <c r="D224" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="225">
@@ -4499,10 +4499,10 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D225" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="226">
@@ -4520,7 +4520,7 @@
         <v>2</v>
       </c>
       <c r="D226" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="227">
@@ -4535,10 +4535,10 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D227" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="228">
@@ -4553,10 +4553,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D228" s="1" t="n">
-        <v>45321</v>
+        <v>45339</v>
       </c>
     </row>
     <row r="229">
@@ -4571,10 +4571,10 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D229" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="230">
@@ -4592,7 +4592,7 @@
         <v>2</v>
       </c>
       <c r="D230" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="231">
@@ -4613,7 +4613,7 @@
         <v>1</v>
       </c>
       <c r="D231" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="232">
@@ -4631,7 +4631,7 @@
         <v>1</v>
       </c>
       <c r="D232" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="233">
@@ -4646,10 +4646,10 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D233" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="234">
@@ -4667,7 +4667,7 @@
         <v>1</v>
       </c>
       <c r="D234" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="235">
@@ -4683,10 +4683,10 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D235" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="236">
@@ -4701,10 +4701,10 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D236" s="1" t="n">
-        <v>45323</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="237">
@@ -4722,7 +4722,7 @@
         <v>1</v>
       </c>
       <c r="D237" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="238">
@@ -4737,10 +4737,10 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D238" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="239">
@@ -4755,10 +4755,10 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D239" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="240">
@@ -4776,7 +4776,7 @@
         <v>4</v>
       </c>
       <c r="D240" s="1" t="n">
-        <v>45324</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="241">
@@ -4791,10 +4791,10 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D241" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="242">
@@ -4809,10 +4809,10 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D242" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="243">
@@ -4827,10 +4827,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D243" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="244">
@@ -4849,7 +4849,7 @@
         <v>1</v>
       </c>
       <c r="D244" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="245">
@@ -4867,7 +4867,7 @@
         <v>1</v>
       </c>
       <c r="D245" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="246">
@@ -4882,10 +4882,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D246" s="1" t="n">
-        <v>45320</v>
+        <v>45339</v>
       </c>
     </row>
     <row r="247">
@@ -4903,7 +4903,7 @@
         <v>1</v>
       </c>
       <c r="D247" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="248">
@@ -4921,7 +4921,7 @@
         <v>1</v>
       </c>
       <c r="D248" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="249">
@@ -4939,7 +4939,7 @@
         <v>1</v>
       </c>
       <c r="D249" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="250">
@@ -4957,7 +4957,7 @@
         <v>1</v>
       </c>
       <c r="D250" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="251">
@@ -4975,7 +4975,7 @@
         <v>4</v>
       </c>
       <c r="D251" s="1" t="n">
-        <v>45324</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="252">
@@ -4994,7 +4994,7 @@
         <v>1</v>
       </c>
       <c r="D252" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="253">
@@ -5011,10 +5011,10 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D253" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="254">
@@ -5032,7 +5032,7 @@
         <v>1</v>
       </c>
       <c r="D254" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="255">
@@ -5047,10 +5047,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D255" s="1" t="n">
-        <v>45320</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="256">
@@ -5065,10 +5065,10 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D256" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="257">
@@ -5086,7 +5086,7 @@
         <v>1</v>
       </c>
       <c r="D257" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="258">
@@ -5104,7 +5104,7 @@
         <v>1</v>
       </c>
       <c r="D258" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="259">
@@ -5119,10 +5119,10 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D259" s="1" t="n">
-        <v>45320</v>
+        <v>45340</v>
       </c>
     </row>
     <row r="260">
@@ -5140,7 +5140,7 @@
         <v>2</v>
       </c>
       <c r="D260" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="261">
@@ -5155,10 +5155,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D261" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="262">
@@ -5176,7 +5176,7 @@
         <v>1</v>
       </c>
       <c r="D262" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="263">
@@ -5194,7 +5194,7 @@
         <v>1</v>
       </c>
       <c r="D263" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="264">
@@ -5212,7 +5212,7 @@
         <v>1</v>
       </c>
       <c r="D264" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="265">
@@ -5227,10 +5227,10 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D265" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="266">
@@ -5245,10 +5245,10 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D266" s="1" t="n">
-        <v>45320</v>
+        <v>45340</v>
       </c>
     </row>
     <row r="267">
@@ -5263,10 +5263,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D267" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="268">
@@ -5281,10 +5281,10 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D268" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="269">
@@ -5302,7 +5302,7 @@
         <v>1</v>
       </c>
       <c r="D269" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="270">
@@ -5318,10 +5318,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D270" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="271">
@@ -5336,10 +5336,10 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D271" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="272">
@@ -5357,7 +5357,7 @@
         <v>1</v>
       </c>
       <c r="D272" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="273">
@@ -5375,7 +5375,7 @@
         <v>1</v>
       </c>
       <c r="D273" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="274">
@@ -5393,7 +5393,7 @@
         <v>1</v>
       </c>
       <c r="D274" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="275">
@@ -5411,7 +5411,7 @@
         <v>1</v>
       </c>
       <c r="D275" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="276">
@@ -5429,7 +5429,7 @@
         <v>1</v>
       </c>
       <c r="D276" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="277">
@@ -5448,7 +5448,7 @@
         <v>1</v>
       </c>
       <c r="D277" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="278">
@@ -5467,7 +5467,7 @@
         <v>1</v>
       </c>
       <c r="D278" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="279">
@@ -5486,7 +5486,7 @@
         <v>1</v>
       </c>
       <c r="D279" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="280">
@@ -5501,10 +5501,10 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D280" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="281">
@@ -5522,7 +5522,7 @@
         <v>1</v>
       </c>
       <c r="D281" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="282">
@@ -5540,7 +5540,7 @@
         <v>1</v>
       </c>
       <c r="D282" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="283">
@@ -5559,7 +5559,7 @@
         <v>1</v>
       </c>
       <c r="D283" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="284">
@@ -5578,7 +5578,7 @@
         <v>2</v>
       </c>
       <c r="D284" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="285">
@@ -5595,10 +5595,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D285" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="286">
@@ -5618,7 +5618,7 @@
         <v>1</v>
       </c>
       <c r="D286" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="287">
@@ -5636,7 +5636,7 @@
         <v>1</v>
       </c>
       <c r="D287" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="288">
@@ -5652,10 +5652,10 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D288" s="1" t="n">
-        <v>45320</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="289">
@@ -5673,7 +5673,7 @@
         <v>1</v>
       </c>
       <c r="D289" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="290">
@@ -5691,7 +5691,7 @@
         <v>1</v>
       </c>
       <c r="D290" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="291">
@@ -5709,7 +5709,7 @@
         <v>1</v>
       </c>
       <c r="D291" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="292">
@@ -5728,7 +5728,7 @@
         <v>1</v>
       </c>
       <c r="D292" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="293">
@@ -5747,7 +5747,7 @@
         <v>2</v>
       </c>
       <c r="D293" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="294">
@@ -5766,7 +5766,7 @@
         <v>1</v>
       </c>
       <c r="D294" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="295">
@@ -5784,7 +5784,7 @@
         <v>1</v>
       </c>
       <c r="D295" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="296">
@@ -5802,7 +5802,7 @@
         <v>1</v>
       </c>
       <c r="D296" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="297">
@@ -5817,10 +5817,10 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D297" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="298">
@@ -5838,7 +5838,7 @@
         <v>1</v>
       </c>
       <c r="D298" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="299">
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D299" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="300">
@@ -5873,10 +5873,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D300" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="301">
@@ -5894,7 +5894,7 @@
         <v>1</v>
       </c>
       <c r="D301" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="302">
@@ -5912,7 +5912,7 @@
         <v>1</v>
       </c>
       <c r="D302" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="303">
@@ -5928,10 +5928,10 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D303" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="304">
@@ -5950,7 +5950,7 @@
         <v>1</v>
       </c>
       <c r="D304" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="305">
@@ -5969,7 +5969,7 @@
         <v>1</v>
       </c>
       <c r="D305" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="306">
@@ -5987,7 +5987,7 @@
         <v>1</v>
       </c>
       <c r="D306" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="307">
@@ -6005,7 +6005,7 @@
         <v>1</v>
       </c>
       <c r="D307" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="308">
@@ -6023,7 +6023,7 @@
         <v>1</v>
       </c>
       <c r="D308" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="309">
@@ -6039,10 +6039,10 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D309" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="310">
@@ -6057,10 +6057,10 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D310" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="311">
@@ -6080,7 +6080,7 @@
         <v>1</v>
       </c>
       <c r="D311" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="312">
@@ -6097,10 +6097,10 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D312" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="313">
@@ -6119,7 +6119,7 @@
         <v>2</v>
       </c>
       <c r="D313" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="314">
@@ -6137,10 +6137,10 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D314" s="1" t="n">
-        <v>45320</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="315">
@@ -6157,10 +6157,10 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D315" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="316">
@@ -6176,10 +6176,10 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D316" s="1" t="n">
-        <v>45320</v>
+        <v>45339</v>
       </c>
     </row>
     <row r="317">
@@ -6197,7 +6197,7 @@
         <v>1</v>
       </c>
       <c r="D317" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="318">
@@ -6217,7 +6217,7 @@
         <v>1</v>
       </c>
       <c r="D318" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="319">
@@ -6233,10 +6233,10 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D319" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="320">
@@ -6256,7 +6256,7 @@
         <v>1</v>
       </c>
       <c r="D320" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="321">
@@ -6275,10 +6275,10 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D321" s="1" t="n">
-        <v>45320</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="322">
@@ -6297,7 +6297,7 @@
         <v>1</v>
       </c>
       <c r="D322" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="323">
@@ -6315,7 +6315,7 @@
         <v>1</v>
       </c>
       <c r="D323" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="324">
@@ -6332,10 +6332,10 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D324" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="325">
@@ -6351,10 +6351,10 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D325" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="326">
@@ -6373,7 +6373,7 @@
         <v>1</v>
       </c>
       <c r="D326" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="327">
@@ -6392,7 +6392,7 @@
         <v>1</v>
       </c>
       <c r="D327" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="328">
@@ -6410,7 +6410,7 @@
         <v>1</v>
       </c>
       <c r="D328" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="329">
@@ -6428,7 +6428,7 @@
         <v>1</v>
       </c>
       <c r="D329" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="330">
@@ -6447,7 +6447,7 @@
         <v>1</v>
       </c>
       <c r="D330" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="331">
@@ -6462,10 +6462,10 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D331" s="1" t="n">
-        <v>45320</v>
+        <v>45339</v>
       </c>
     </row>
     <row r="332">
@@ -6484,7 +6484,7 @@
         <v>1</v>
       </c>
       <c r="D332" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="333">
@@ -6499,10 +6499,10 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D333" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="334">
@@ -6521,7 +6521,7 @@
         <v>1</v>
       </c>
       <c r="D334" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="335">
@@ -6539,7 +6539,7 @@
         <v>1</v>
       </c>
       <c r="D335" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="336">
@@ -6557,7 +6557,7 @@
         <v>2</v>
       </c>
       <c r="D336" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="337">
@@ -6577,7 +6577,7 @@
         <v>1</v>
       </c>
       <c r="D337" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="338">
@@ -6595,7 +6595,7 @@
         <v>1</v>
       </c>
       <c r="D338" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="339">
@@ -6610,10 +6610,10 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D339" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="340">
@@ -6631,7 +6631,7 @@
         <v>2</v>
       </c>
       <c r="D340" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="341">
@@ -6646,10 +6646,10 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D341" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="342">
@@ -6664,10 +6664,10 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D342" s="1" t="n">
-        <v>45322</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="343">
@@ -6685,7 +6685,7 @@
         <v>2</v>
       </c>
       <c r="D343" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="344">
@@ -6706,7 +6706,7 @@
         <v>2</v>
       </c>
       <c r="D344" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="345">
@@ -6722,10 +6722,10 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D345" s="1" t="n">
-        <v>45320</v>
+        <v>45339</v>
       </c>
     </row>
     <row r="346">
@@ -6743,7 +6743,7 @@
         <v>1</v>
       </c>
       <c r="D346" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="347">
@@ -6764,7 +6764,7 @@
         <v>1</v>
       </c>
       <c r="D347" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="348">
@@ -6779,10 +6779,10 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D348" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="349">
@@ -6800,7 +6800,7 @@
         <v>1</v>
       </c>
       <c r="D349" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="350">
@@ -6817,10 +6817,10 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D350" s="1" t="n">
-        <v>45320</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="351">
@@ -6838,7 +6838,7 @@
         <v>1</v>
       </c>
       <c r="D351" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="352">
@@ -6856,7 +6856,7 @@
         <v>1</v>
       </c>
       <c r="D352" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="353">
@@ -6871,10 +6871,10 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D353" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="354">
@@ -6889,10 +6889,10 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D354" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="355">
@@ -6910,7 +6910,7 @@
         <v>1</v>
       </c>
       <c r="D355" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="356">
@@ -6926,10 +6926,10 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D356" s="1" t="n">
-        <v>45320</v>
+        <v>45340</v>
       </c>
     </row>
     <row r="357">
@@ -6947,7 +6947,7 @@
         <v>1</v>
       </c>
       <c r="D357" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="358">
@@ -6964,10 +6964,10 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D358" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="359">
@@ -6986,7 +6986,7 @@
         <v>1</v>
       </c>
       <c r="D359" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="360">
@@ -7001,10 +7001,10 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D360" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="361">
@@ -7022,7 +7022,7 @@
         <v>1</v>
       </c>
       <c r="D361" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="362">
@@ -7037,10 +7037,10 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D362" s="1" t="n">
-        <v>45320</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="363">
@@ -7058,7 +7058,7 @@
         <v>1</v>
       </c>
       <c r="D363" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="364">
@@ -7079,7 +7079,7 @@
         <v>1</v>
       </c>
       <c r="D364" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="365">
@@ -7097,7 +7097,7 @@
         <v>1</v>
       </c>
       <c r="D365" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="366">
@@ -7117,7 +7117,7 @@
         <v>1</v>
       </c>
       <c r="D366" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="367">
@@ -7136,7 +7136,7 @@
         <v>2</v>
       </c>
       <c r="D367" s="1" t="n">
-        <v>45321</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="368">
@@ -7154,7 +7154,7 @@
         <v>1</v>
       </c>
       <c r="D368" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="369">
@@ -7171,10 +7171,10 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D369" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="370">
@@ -7194,7 +7194,7 @@
         <v>1</v>
       </c>
       <c r="D370" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="371">
@@ -7213,7 +7213,7 @@
         <v>1</v>
       </c>
       <c r="D371" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="372">
@@ -7228,10 +7228,10 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D372" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="373">
@@ -7246,10 +7246,10 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D373" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="374">
@@ -7264,10 +7264,10 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D374" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="375">
@@ -7286,7 +7286,7 @@
         <v>1</v>
       </c>
       <c r="D375" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="376">
@@ -7304,7 +7304,7 @@
         <v>1</v>
       </c>
       <c r="D376" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="377">
@@ -7324,7 +7324,7 @@
         <v>1</v>
       </c>
       <c r="D377" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="378">
@@ -7339,10 +7339,10 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D378" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="379">
@@ -7361,7 +7361,7 @@
         <v>1</v>
       </c>
       <c r="D379" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="380">
@@ -7379,7 +7379,7 @@
         <v>1</v>
       </c>
       <c r="D380" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="381">
@@ -7397,7 +7397,7 @@
         <v>1</v>
       </c>
       <c r="D381" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="382">
@@ -7412,10 +7412,10 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D382" s="1" t="n">
-        <v>45320</v>
+        <v>45337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>